<commit_message>
OCP Coding Challenge: Task 2
</commit_message>
<xml_diff>
--- a/doc/valid_barcodes.xlsx
+++ b/doc/valid_barcodes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Barcode</t>
   </si>
@@ -24,26 +24,35 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>00000079</t>
+    <t>00000314</t>
   </si>
   <si>
     <t>valid</t>
   </si>
   <si>
-    <t>00000093</t>
+    <t>1234567</t>
   </si>
   <si>
-    <t>00000314</t>
+    <t>append calculated checksum</t>
   </si>
   <si>
-    <t>12345670</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>pad and append calculated checksum</t>
+  </si>
+  <si>
+    <t>00031</t>
+  </si>
+  <si>
+    <t>pad only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -58,6 +67,12 @@
       <sz val="10.0"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -67,13 +82,27 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -83,8 +112,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,10 +379,10 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1"/>
@@ -373,11 +411,11 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -405,11 +443,11 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -438,10 +476,10 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -470,219 +508,219 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>

</xml_diff>